<commit_message>
before removing a great part of the datasets
</commit_message>
<xml_diff>
--- a/merlin_discord_results.xlsx
+++ b/merlin_discord_results.xlsx
@@ -518,11 +518,11 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>{'cluster': 16, 'training': 1329, 'window': 200, 'threshold': 3.0}</t>
+          <t>{'cluster': 15, 'training': 1330, 'window': 200, 'threshold': 8.0}</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0.2120239068754017</v>
+        <v>0.5077524951193482</v>
       </c>
     </row>
     <row r="3">
@@ -550,7 +550,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[1600, 1700, 1800, 4000, 4100, 4200, 4400, 4500, 4600, 4700, 4800, 4900]</t>
+          <t>[1600, 1700, 1800, 4000, 4100, 4200, 4400, 4500, 4700, 4800, 4900]</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -558,11 +558,11 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>{'cluster': 14, 'training': 1177, 'window': 200, 'threshold': 1.5}</t>
+          <t>{'cluster': 14, 'training': 1256, 'window': 200, 'threshold': 2.5}</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>0.2517397562041879</v>
+        <v>0.7068190251011401</v>
       </c>
     </row>
     <row r="4">
@@ -598,11 +598,11 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>{'cluster': 12, 'training': 1204, 'window': 200, 'threshold': 1.0}</t>
+          <t>{'cluster': 16, 'training': 1236, 'window': 200, 'threshold': 4.5}</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0.2564647619146854</v>
+        <v>0.8544361060485244</v>
       </c>
     </row>
     <row r="5">
@@ -638,11 +638,11 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>{'cluster': 23, 'training': 704, 'window': 200, 'threshold': 9.5}</t>
+          <t>{'cluster': 17, 'training': 751, 'window': 200, 'threshold': 2.5}</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>0.1048812088556588</v>
+        <v>0.5201737459283322</v>
       </c>
     </row>
     <row r="6">
@@ -678,11 +678,11 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>{'cluster': 20, 'training': 738, 'window': 200, 'threshold': 4.0}</t>
+          <t>{'cluster': 19, 'training': 440, 'window': 200, 'threshold': 3.0}</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0.1179139178711921</v>
+        <v>0.4550081070046872</v>
       </c>
     </row>
     <row r="7">
@@ -712,19 +712,19 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>[10500, 10800]</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>0.4762962962962962</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>params</t>
+          <t>{'cluster': 10, 'training': 4479, 'window': 600, 'threshold': 3.5}</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>0.4726196799892932</v>
       </c>
     </row>
     <row r="8">
@@ -752,19 +752,19 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>[340, 360, 380, 740, 820, 1080, 1140, 1240, 1260, 1540, 1660, 1860, 1960, 2040, 2560, 2580, 2880, 3160, 3440, 4000, 4060, 4140, 4160, 4360, 4500, 4800, 5280, 5340, 5420, 5640, 5660, 5760, 5940, 6240, 6440, 6520, 6640, 6740, 6840, 6860, 6880, 6900, 6920, 7040, 7460, 7520, 7640, 7920, 7960, 8560, 8780, 8860, 8940, 9200, 9300, 9320, 9340, 9440, 9740, 9760, 10040, 10060, 10180, 10200, 10460, 10480, 11040, 11060, 11400, 11660, 11680, 11880, 11940, 12300, 12480, 12660, 12720, 12920, 12960, 12980, 13100, 13120, 13160, 13560, 13620, 13760, 13880, 14100, 14120, 14140, 14220, 14260, 14280, 14360, 14400, 14420, 14480, 14780, 14900]</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>0.01704545454545455</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>params</t>
+          <t>{'cluster': 10, 'training': 222, 'window': 40, 'threshold': 4.5}</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>4.840415807906538</v>
       </c>
     </row>
     <row r="9">
@@ -792,19 +792,19 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>[2300, 4800]</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>params</t>
+          <t>{'cluster': 15, 'training': 2915, 'window': 200, 'threshold': 1.5}</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>2.022873396985233</v>
       </c>
     </row>
     <row r="10">
@@ -832,19 +832,19 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>[300, 375, 2100, 2175, 2250, 2325, 2400]</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>params</t>
+          <t>{'cluster': 13, 'training': 178, 'window': 150, 'threshold': 1.0}</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>2.639962041983381</v>
       </c>
     </row>
     <row r="11">
@@ -874,19 +874,19 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>[5000]</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>params</t>
+          <t>{'cluster': 14, 'training': 1011, 'window': 100, 'threshold': 4.5}</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>3.780867037829012</v>
       </c>
     </row>
     <row r="12">
@@ -958,19 +958,19 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>[4392, 4758, 4941, 6588, 6771, 12810]</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>0.2857142857142858</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>params</t>
+          <t>{'cluster': 18, 'training': 4210, 'window': 366, 'threshold': 8.5}</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>0.8104959439951926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>